<commit_message>
Added hopscotch to individual benchmark. Updated cache chart.
</commit_message>
<xml_diff>
--- a/charts/cache_performance.xlsx
+++ b/charts/cache_performance.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>C++11 Unordered Map</t>
   </si>
@@ -42,13 +42,25 @@
     <t>Cuckoo w/ Multiplication</t>
   </si>
   <si>
-    <t>Cache Probes</t>
-  </si>
-  <si>
     <t>Cache Misses</t>
   </si>
   <si>
     <t>Hit Rate</t>
+  </si>
+  <si>
+    <t>Hopscotch w/ Tabulation</t>
+  </si>
+  <si>
+    <t>Hopscotch w/ Multiplication</t>
+  </si>
+  <si>
+    <t>Misses/Query</t>
+  </si>
+  <si>
+    <t>Cache References</t>
+  </si>
+  <si>
+    <t>Ref/query</t>
   </si>
 </sst>
 </file>
@@ -130,11 +142,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cache Probes</c:v>
+                  <c:v>Ref/query</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -142,9 +154,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -164,9 +176,15 @@
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Hopscotch w/ Tabulation</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hopscotch w/ Multiplication</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -174,33 +192,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12524183</c:v>
+                  <c:v>11.321788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12542625</c:v>
+                  <c:v>11.465168999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7461729</c:v>
+                  <c:v>7.6177250000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7355928</c:v>
+                  <c:v>7.6236879999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8130107</c:v>
+                  <c:v>8.4345820000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8122182</c:v>
+                  <c:v>8.3427170000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10267162</c:v>
+                  <c:v>7.607183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10115003</c:v>
+                  <c:v>7.5209450000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.178357</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.449630000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -215,11 +239,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="70069248"/>
-        <c:axId val="73076736"/>
+        <c:axId val="106224256"/>
+        <c:axId val="106537344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70069248"/>
+        <c:axId val="106224256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -228,7 +252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73076736"/>
+        <c:crossAx val="106537344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -236,10 +260,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73076736"/>
+        <c:axId val="106537344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -248,7 +271,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70069248"/>
+        <c:crossAx val="106224256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -295,11 +318,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cache Misses</c:v>
+                  <c:v>Misses/Query</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -307,9 +330,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -329,9 +352,15 @@
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Hopscotch w/ Tabulation</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hopscotch w/ Multiplication</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -339,33 +368,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6109007</c:v>
+                  <c:v>5.3557579999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6657201</c:v>
+                  <c:v>5.9774609999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3973427</c:v>
+                  <c:v>2.1981419999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3934201</c:v>
+                  <c:v>2.1732390000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4324954</c:v>
+                  <c:v>2.2879800000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4322246</c:v>
+                  <c:v>2.261971</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6283020</c:v>
+                  <c:v>2.2016810000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6241723</c:v>
+                  <c:v>2.132959</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3756529999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.417821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -380,20 +415,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="113270144"/>
-        <c:axId val="113304704"/>
+        <c:axId val="106565632"/>
+        <c:axId val="106567168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113270144"/>
+        <c:axId val="106565632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113304704"/>
+        <c:crossAx val="106567168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -401,10 +437,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113304704"/>
+        <c:axId val="106567168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="3000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -413,7 +448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113270144"/>
+        <c:crossAx val="106565632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -460,7 +495,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -472,9 +507,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -494,9 +529,15 @@
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Hopscotch w/ Tabulation</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hopscotch w/ Multiplication</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -504,33 +545,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.51222311267729004</c:v>
+                  <c:v>0.52695122007230655</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46923383263072926</c:v>
+                  <c:v>0.47864170166178976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46749245382672033</c:v>
+                  <c:v>0.71144377094211197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46516591788282868</c:v>
+                  <c:v>0.71493599947951703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46803233954977463</c:v>
+                  <c:v>0.7287381876185447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46784669439813098</c:v>
+                  <c:v>0.728868784593796</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.38804705721016186</c:v>
+                  <c:v>0.71057867281489084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38292425617669124</c:v>
+                  <c:v>0.71639747398764386</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.77760089580183145</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76346653858956937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -545,11 +592,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116438912"/>
-        <c:axId val="116440448"/>
+        <c:axId val="106620032"/>
+        <c:axId val="106621568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116438912"/>
+        <c:axId val="106620032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -558,7 +605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116440448"/>
+        <c:crossAx val="106621568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -566,10 +613,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116440448"/>
+        <c:axId val="106621568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -578,7 +624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116438912"/>
+        <c:crossAx val="106620032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -599,16 +645,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681037</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -629,16 +675,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42862</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>938212</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -659,16 +705,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>433387</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -977,149 +1023,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="D1:D9 A1:A9"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12524183</v>
+        <v>11321788</v>
       </c>
       <c r="C2">
-        <v>6109007</v>
+        <f>B2/1000000</f>
+        <v>11.321788</v>
       </c>
       <c r="D2">
-        <f>1 - C2/B2</f>
-        <v>0.51222311267729004</v>
+        <v>5355758</v>
+      </c>
+      <c r="E2">
+        <f>D2/1000000</f>
+        <v>5.3557579999999998</v>
+      </c>
+      <c r="F2">
+        <f>1 - D2/B2</f>
+        <v>0.52695122007230655</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>12542625</v>
+        <v>11465169</v>
       </c>
       <c r="C3">
-        <v>6657201</v>
+        <f t="shared" ref="C3:C11" si="0">B3/1000000</f>
+        <v>11.465168999999999</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">1 - C3/B3</f>
-        <v>0.46923383263072926</v>
+        <v>5977461</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="1">D3/1000000</f>
+        <v>5.9774609999999999</v>
+      </c>
+      <c r="F3">
+        <f>1 - D3/B3</f>
+        <v>0.47864170166178976</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7461729</v>
+        <v>7617725</v>
       </c>
       <c r="C4">
-        <v>3973427</v>
+        <f t="shared" si="0"/>
+        <v>7.6177250000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.46749245382672033</v>
+        <v>2198142</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>2.1981419999999998</v>
+      </c>
+      <c r="F4">
+        <f>1 - D4/B4</f>
+        <v>0.71144377094211197</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7355928</v>
+        <v>7623688</v>
       </c>
       <c r="C5">
-        <v>3934201</v>
+        <f t="shared" si="0"/>
+        <v>7.6236879999999996</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.46516591788282868</v>
+        <v>2173239</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.1732390000000001</v>
+      </c>
+      <c r="F5">
+        <f>1 - D5/B5</f>
+        <v>0.71493599947951703</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>8130107</v>
+        <v>8434582</v>
       </c>
       <c r="C6">
-        <v>4324954</v>
+        <f t="shared" si="0"/>
+        <v>8.4345820000000007</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.46803233954977463</v>
+        <v>2287980</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2.2879800000000001</v>
+      </c>
+      <c r="F6">
+        <f>1 - D6/B6</f>
+        <v>0.7287381876185447</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8122182</v>
+        <v>8342717</v>
       </c>
       <c r="C7">
-        <v>4322246</v>
+        <f t="shared" si="0"/>
+        <v>8.3427170000000004</v>
       </c>
       <c r="D7">
+        <v>2261971</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>2.261971</v>
+      </c>
+      <c r="F7">
+        <f>1 - D7/B7</f>
+        <v>0.728868784593796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>7607183</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.46784669439813098</v>
+        <v>7.607183</v>
+      </c>
+      <c r="D8">
+        <v>2201681</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2.2016810000000002</v>
+      </c>
+      <c r="F8">
+        <f>1 - D8/B8</f>
+        <v>0.71057867281489084</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>7520945</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>7.5209450000000002</v>
+      </c>
+      <c r="D9">
+        <v>2132959</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2.132959</v>
+      </c>
+      <c r="F9">
+        <f>1 - D9/B9</f>
+        <v>0.71639747398764386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>10267162</v>
-      </c>
-      <c r="C8">
-        <v>6283020</v>
-      </c>
-      <c r="D8">
+      <c r="B10">
+        <v>15178357</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.38804705721016186</v>
+        <v>15.178357</v>
+      </c>
+      <c r="D10">
+        <v>3375653</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>3.3756529999999998</v>
+      </c>
+      <c r="F10">
+        <f>1 - D10/B10</f>
+        <v>0.77760089580183145</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>10115003</v>
-      </c>
-      <c r="C9">
-        <v>6241723</v>
-      </c>
-      <c r="D9">
+      <c r="B11">
+        <v>14449630</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.38292425617669124</v>
+        <v>14.449630000000001</v>
+      </c>
+      <c r="D11">
+        <v>3417821</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>3.417821</v>
+      </c>
+      <c r="F11">
+        <f>1 - D11/B11</f>
+        <v>0.76346653858956937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prettified code. Added boost to cache and overall performance charts.
</commit_message>
<xml_diff>
--- a/charts/cache_performance.xlsx
+++ b/charts/cache_performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>C++11 Unordered Map</t>
   </si>
@@ -65,15 +65,28 @@
   <si>
     <t>Running time</t>
   </si>
+  <si>
+    <t>DON'T USE THIS CHART!</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="25"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,6 +144,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -241,11 +256,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="71753728"/>
-        <c:axId val="71755264"/>
+        <c:axId val="84463616"/>
+        <c:axId val="84465152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71753728"/>
+        <c:axId val="84463616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,7 +269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71755264"/>
+        <c:crossAx val="84465152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -262,7 +277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71755264"/>
+        <c:axId val="84465152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -273,7 +288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71753728"/>
+        <c:crossAx val="84463616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -305,6 +320,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -416,11 +432,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="85851136"/>
-        <c:axId val="86222336"/>
+        <c:axId val="85881984"/>
+        <c:axId val="85883520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85851136"/>
+        <c:axId val="85881984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86222336"/>
+        <c:crossAx val="85883520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -438,7 +454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86222336"/>
+        <c:axId val="85883520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85851136"/>
+        <c:crossAx val="85881984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -481,6 +497,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -592,11 +609,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="93734400"/>
-        <c:axId val="93735936"/>
+        <c:axId val="85903616"/>
+        <c:axId val="85909504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93734400"/>
+        <c:axId val="85903616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93735936"/>
+        <c:crossAx val="85909504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -613,7 +630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93735936"/>
+        <c:axId val="85909504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -624,7 +641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93734400"/>
+        <c:crossAx val="85903616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -683,9 +700,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'9x read'!$A$2:$A$11</c:f>
+              <c:f>'9x read'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -693,27 +710,30 @@
                   <c:v>GCC/ext Hash Map</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Boost</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Linear Probing w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Linear Probing w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Quadratic w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Hopscotch w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Hopscotch w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -721,39 +741,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9x read'!$C$2:$C$11</c:f>
+              <c:f>'9x read'!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3.790616111111111</c:v>
+                  <c:v>3.8284771111111113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.054686666666667</c:v>
+                  <c:v>4.0453965555555556</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6967647777777777</c:v>
+                  <c:v>4.0407279999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6754453333333332</c:v>
+                  <c:v>3.772788888888889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3743613333333338</c:v>
+                  <c:v>3.6985545555555555</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2920631111111112</c:v>
+                  <c:v>4.3109394444444442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.7046117777777776</c:v>
+                  <c:v>4.3160660000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6449498888888887</c:v>
+                  <c:v>3.6898056666666665</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4035842222222223</c:v>
+                  <c:v>3.6304132222222223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2254440000000004</c:v>
+                  <c:v>6.4255121111111109</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1203598888888893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,11 +791,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="138903936"/>
-        <c:axId val="138905856"/>
+        <c:axId val="91848704"/>
+        <c:axId val="91850240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138903936"/>
+        <c:axId val="91848704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,7 +804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138905856"/>
+        <c:crossAx val="91850240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -789,7 +812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138905856"/>
+        <c:axId val="91850240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138903936"/>
+        <c:crossAx val="91848704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -859,9 +882,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'9x read'!$A$2:$A$11</c:f>
+              <c:f>'9x read'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -869,27 +892,30 @@
                   <c:v>GCC/ext Hash Map</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Boost</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Linear Probing w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Linear Probing w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Quadratic w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Hopscotch w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Hopscotch w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -897,39 +923,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9x read'!$E$2:$E$11</c:f>
+              <c:f>'9x read'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.0545674444444444</c:v>
+                  <c:v>2.0557855555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3619072222222224</c:v>
+                  <c:v>2.3590151111111113</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99108666666666667</c:v>
+                  <c:v>2.3645185555555557</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98909477777777777</c:v>
+                  <c:v>0.97975611111111116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.066632</c:v>
+                  <c:v>0.98601444444444442</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0935625555555555</c:v>
+                  <c:v>1.0644006666666668</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98048388888888893</c:v>
+                  <c:v>1.0748498888888889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97498433333333334</c:v>
+                  <c:v>0.98411966666666661</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3546590000000001</c:v>
+                  <c:v>0.96860477777777776</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1334766666666667</c:v>
+                  <c:v>1.3730566666666666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3137126666666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -944,11 +973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5282816"/>
-        <c:axId val="5288704"/>
+        <c:axId val="91867776"/>
+        <c:axId val="92148096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5282816"/>
+        <c:axId val="91867776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +987,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5288704"/>
+        <c:crossAx val="92148096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -966,7 +995,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5288704"/>
+        <c:axId val="92148096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +1006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5282816"/>
+        <c:crossAx val="91867776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1036,9 +1065,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'9x read'!$A$2:$A$11</c:f>
+              <c:f>'9x read'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -1046,27 +1075,30 @@
                   <c:v>GCC/ext Hash Map</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Boost</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Linear Probing w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Linear Probing w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Quadratic w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Hopscotch w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Hopscotch w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1074,39 +1106,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9x read'!$F$2:$F$11</c:f>
+              <c:f>'9x read'!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.4579858829750485</c:v>
+                  <c:v>0.4630278578421696</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41748711641781888</c:v>
+                  <c:v>0.41686431015731484</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73190432006268069</c:v>
+                  <c:v>0.4148285765447326</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73089117424561223</c:v>
+                  <c:v>0.74030985036121233</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75616280441396244</c:v>
+                  <c:v>0.73340546161111408</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74521284351001571</c:v>
+                  <c:v>0.75309310641364458</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73533424075085274</c:v>
+                  <c:v>0.75096537242737049</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73251090877670655</c:v>
+                  <c:v>0.73328685693203166</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78845300491263071</c:v>
+                  <c:v>0.73319709947924816</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78308509924387926</c:v>
+                  <c:v>0.78631171447138781</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.78535368989467014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,11 +1156,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5304704"/>
-        <c:axId val="5306240"/>
+        <c:axId val="92168576"/>
+        <c:axId val="92170112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5304704"/>
+        <c:axId val="92168576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +1169,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5306240"/>
+        <c:crossAx val="92170112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1142,7 +1177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5306240"/>
+        <c:axId val="92170112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,7 +1188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5304704"/>
+        <c:crossAx val="92168576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1227,9 +1262,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'9x read'!$A$2:$A$11</c:f>
+              <c:f>'9x read'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>C++11 Unordered Map</c:v>
                 </c:pt>
@@ -1237,27 +1272,30 @@
                   <c:v>GCC/ext Hash Map</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Boost</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Linear Probing w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Linear Probing w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Quadratic w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Quadratic w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Hopscotch w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Hopscotch w/ Multiplication</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Cuckoo w/ Tabulation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Cuckoo w/ Multiplication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1265,39 +1303,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'9x read'!$G$2:$G$11</c:f>
+              <c:f>'9x read'!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.0132565950000001</c:v>
+                  <c:v>2.4648759999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2515231120000001</c:v>
+                  <c:v>2.084562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4053546969999999</c:v>
+                  <c:v>2.4025789999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2767588459999999</c:v>
+                  <c:v>1.3668750000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.496755466</c:v>
+                  <c:v>1.101121</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2486401600000001</c:v>
+                  <c:v>1.46123</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4101760679999999</c:v>
+                  <c:v>1.370069</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.143006441</c:v>
+                  <c:v>1.3612880000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1063770470000001</c:v>
+                  <c:v>1.1102970000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.944745363</c:v>
+                  <c:v>3.3966859999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.176183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,11 +1353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="88235392"/>
-        <c:axId val="88253568"/>
+        <c:axId val="92190208"/>
+        <c:axId val="92191744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88235392"/>
+        <c:axId val="92190208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1326,7 +1367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88253568"/>
+        <c:crossAx val="92191744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1334,7 +1375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88253568"/>
+        <c:axId val="92191744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,7 +1386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88235392"/>
+        <c:crossAx val="92190208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1877,13 +1918,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1892,7 +1931,10 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -2141,16 +2183,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,25 +2232,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>34115545</v>
+        <v>34456294</v>
       </c>
       <c r="C2">
         <f>B2/9000000</f>
-        <v>3.790616111111111</v>
+        <v>3.8284771111111113</v>
       </c>
       <c r="D2">
-        <v>18491107</v>
+        <v>18502070</v>
       </c>
       <c r="E2">
         <f>D2/9000000</f>
-        <v>2.0545674444444444</v>
+        <v>2.0557855555555555</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F11" si="0">1 - D2/B2</f>
-        <v>0.4579858829750485</v>
+        <f t="shared" ref="F2:F12" si="0">1 - D2/B2</f>
+        <v>0.4630278578421696</v>
       </c>
       <c r="G2">
-        <v>2.0132565950000001</v>
+        <v>2.4648759999999998</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2215,233 +2258,259 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>36492180</v>
+        <v>36408569</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="1">B3/9000000</f>
-        <v>4.054686666666667</v>
+        <f t="shared" ref="C3:C12" si="1">B3/9000000</f>
+        <v>4.0453965555555556</v>
       </c>
       <c r="D3">
-        <v>21257165</v>
+        <v>21231136</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="2">D3/9000000</f>
-        <v>2.3619072222222224</v>
+        <f t="shared" ref="E3:E12" si="2">D3/9000000</f>
+        <v>2.3590151111111113</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.41748711641781888</v>
+        <v>0.41686431015731484</v>
       </c>
       <c r="G3">
-        <v>2.2515231120000001</v>
+        <v>2.084562</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>33270883</v>
+        <v>36366552</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>3.6967647777777777</v>
+        <v>4.0407279999999997</v>
       </c>
       <c r="D4">
-        <v>8919780</v>
+        <v>21280667</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>0.99108666666666667</v>
+        <v>2.3645185555555557</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.73190432006268069</v>
+        <v>0.4148285765447326</v>
       </c>
       <c r="G4">
-        <v>1.4053546969999999</v>
+        <v>2.4025789999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>33079008</v>
+        <v>33955100</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>3.6754453333333332</v>
+        <v>3.772788888888889</v>
       </c>
       <c r="D5">
-        <v>8901853</v>
+        <v>8817805</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>0.98909477777777777</v>
+        <v>0.97975611111111116</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.73089117424561223</v>
+        <v>0.74030985036121233</v>
       </c>
       <c r="G5">
-        <v>1.2767588459999999</v>
+        <v>1.3668750000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>39369252</v>
+        <v>33286991</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>4.3743613333333338</v>
+        <v>3.6985545555555555</v>
       </c>
       <c r="D6">
-        <v>9599688</v>
+        <v>8874130</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>1.066632</v>
+        <v>0.98601444444444442</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.75616280441396244</v>
+        <v>0.73340546161111408</v>
       </c>
       <c r="G6">
-        <v>1.496755466</v>
+        <v>1.101121</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>38628568</v>
+        <v>38798455</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>4.2920631111111112</v>
+        <v>4.3109394444444442</v>
       </c>
       <c r="D7">
-        <v>9842063</v>
+        <v>9579606</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>1.0935625555555555</v>
+        <v>1.0644006666666668</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.74521284351001571</v>
+        <v>0.75309310641364458</v>
       </c>
       <c r="G7">
-        <v>1.2486401600000001</v>
+        <v>1.46123</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>33341506</v>
+        <v>38844594</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>3.7046117777777776</v>
+        <v>4.3160660000000002</v>
       </c>
       <c r="D8">
-        <v>8824355</v>
+        <v>9673649</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>0.98048388888888893</v>
+        <v>1.0748498888888889</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0.73533424075085274</v>
+        <v>0.75096537242737049</v>
       </c>
       <c r="G8">
-        <v>1.4101760679999999</v>
+        <v>1.370069</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>32804549</v>
+        <v>33208251</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>3.6449498888888887</v>
+        <v>3.6898056666666665</v>
       </c>
       <c r="D9">
-        <v>8774859</v>
+        <v>8857077</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>0.97498433333333334</v>
+        <v>0.98411966666666661</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0.73251090877670655</v>
+        <v>0.73328685693203166</v>
       </c>
       <c r="G9">
-        <v>1.143006441</v>
+        <v>1.3612880000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>57632258</v>
+        <v>32673719</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>6.4035842222222223</v>
+        <v>3.6304132222222223</v>
       </c>
       <c r="D10">
-        <v>12191931</v>
+        <v>8717443</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>1.3546590000000001</v>
+        <v>0.96860477777777776</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.78845300491263071</v>
+        <v>0.73319709947924816</v>
       </c>
       <c r="G10">
-        <v>3.1063770470000001</v>
+        <v>1.1102970000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>47028996</v>
+        <v>57829609</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>5.2254440000000004</v>
+        <v>6.4255121111111109</v>
       </c>
       <c r="D11">
-        <v>10201290</v>
+        <v>12357510</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>1.1334766666666667</v>
+        <v>1.3730566666666666</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.78308509924387926</v>
+        <v>0.78631171447138781</v>
       </c>
       <c r="G11">
-        <v>1.944745363</v>
+        <v>3.3966859999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>55083239</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>6.1203598888888893</v>
+      </c>
+      <c r="D12">
+        <v>11823414</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>1.3137126666666668</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.78535368989467014</v>
+      </c>
+      <c r="G12">
+        <v>2.176183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>